<commit_message>
Adding plot for Overweight/Obese by Age England
</commit_message>
<xml_diff>
--- a/Data/BMI_Data.xlsx
+++ b/Data/BMI_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/UK-cancer-trends/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{64AD1003-ABC4-4AB3-8CAF-930E44C514A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EED7221-FA38-4DD7-8FED-C7A38BD26346}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{64AD1003-ABC4-4AB3-8CAF-930E44C514A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5A4C80B-2C5D-47FD-B6F0-4BCEB7BB83F0}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="11400" firstSheet="6" activeTab="6" xr2:uid="{4FB50E91-3C14-4DA6-B24A-60521494A793}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="2" activeTab="2" xr2:uid="{4FB50E91-3C14-4DA6-B24A-60521494A793}"/>
   </bookViews>
   <sheets>
     <sheet name="England_Men" sheetId="1" r:id="rId1"/>
@@ -15446,8 +15446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF3A6F23-A14C-44C5-A963-58083556BCD8}">
   <dimension ref="A1:AO83"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21241,7 +21241,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21838,7 +21838,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>

</xml_diff>